<commit_message>
fix insert new column before first to work in linux
</commit_message>
<xml_diff>
--- a/Samples/Worksheet.Parser.Api.Sample/Sample.xlsx
+++ b/Samples/Worksheet.Parser.Api.Sample/Sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\worksheet-parser\Samples\Worksheet.Parser.Sample.Api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\WorkSheetParser\Samples\Worksheet.Parser.Api.Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01EC5CA-3F22-498D-9F9F-B2FBC62E205C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A804F0-CE93-406A-9B6D-04E345195D35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3AB961A-9BCA-4EE4-B408-1517484A7AE5}"/>
   </bookViews>
@@ -404,9 +404,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>